<commit_message>
refactor: modified data files
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/boards/deleteBoard.xlsx
+++ b/src/test/resources/testData/boards/deleteBoard.xlsx
@@ -8,14 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sulekhasharma\TrainingRestAssuredNew\src\test\resources\testData\boards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443ED5EC-9698-4307-B161-727CC8E5EC1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E4EB1F2-43CE-4FEA-888D-10F7D869EE16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="headers" sheetId="1" r:id="rId1"/>
-    <sheet name="pathParams" sheetId="2" r:id="rId2"/>
-    <sheet name="queryParams" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Content-Type</t>
   </si>
@@ -39,24 +37,6 @@
   </si>
   <si>
     <t>*/*</t>
-  </si>
-  <si>
-    <t>key</t>
-  </si>
-  <si>
-    <t>dd486e53123b2dc7d557ce3167040cf6</t>
-  </si>
-  <si>
-    <t>token</t>
-  </si>
-  <si>
-    <t>ATTA07898ac4e95e6b359ac42d39a24124366703106b383b20cd1ab54460fd5b9955F7D3E4FD</t>
-  </si>
-  <si>
-    <t>boardId</t>
-  </si>
-  <si>
-    <t>66c6f3ebcc7465b2d013a4e0</t>
   </si>
 </sst>
 </file>
@@ -92,11 +72,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,7 +356,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -408,64 +385,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13D007AC-5571-49E9-907A-D66184849B72}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1662FD12-1B41-437E-9D38-2954D36A3B8B}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="81.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>